<commit_message>
Updated text visibility and styled it
</commit_message>
<xml_diff>
--- a/uploads/Rasoi_2026-01-10_master_inventory.xlsx
+++ b/uploads/Rasoi_2026-01-10_master_inventory.xlsx
@@ -483,11 +483,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1525,13 +1525,9 @@
           <t>Thai Chilli</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1545,13 +1541,9 @@
           <t>Sattu</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2589,13 +2581,9 @@
           <t>Very Spicy Red Chilli Powder</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B134" t="inlineStr"/>
       <c r="C134" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updated the fields to wrap text
</commit_message>
<xml_diff>
--- a/uploads/Rasoi_2026-01-10_master_inventory.xlsx
+++ b/uploads/Rasoi_2026-01-10_master_inventory.xlsx
@@ -461,13 +461,9 @@
           <t>Onion white</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -481,11 +477,7 @@
           <t>Onion Red</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>0</v>
       </c>
@@ -501,9 +493,13 @@
           <t>Potato Russel</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -773,9 +769,13 @@
           <t>Frozen Peas and carrot cut</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1061,9 +1061,13 @@
           <t>Paneer - Not Appel, not Nanak</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>

</xml_diff>